<commit_message>
finished app server CRUD operations
</commit_message>
<xml_diff>
--- a/design/API Design.xlsx
+++ b/design/API Design.xlsx
@@ -145,7 +145,7 @@
     <t xml:space="preserve">/bookings/id</t>
   </si>
   <si>
-    <t xml:space="preserve">{”roomID":”xxx”,“date”:”xxx”,“userName:”xxx”,”reason”:”xxxx”  }</t>
+    <t xml:space="preserve">{”roomID":”xxx”,“dateRequired”:”xxx”,“userName:”xxx”,”reason”:”xxxx”  }</t>
   </si>
   <si>
     <t xml:space="preserve">Create booking</t>
@@ -169,6 +169,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -285,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,10 +313,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -398,7 +395,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -585,7 +582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -602,7 +599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
@@ -619,7 +616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -636,7 +633,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>32</v>
       </c>
@@ -653,7 +650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -670,7 +667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
@@ -687,7 +684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>39</v>
       </c>
@@ -700,11 +697,11 @@
       <c r="D26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
         <v>42</v>
       </c>
@@ -717,11 +714,11 @@
       <c r="D27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
         <v>43</v>
       </c>

</xml_diff>